<commit_message>
add jpp60  201609 data
</commit_message>
<xml_diff>
--- a/dkjs.git.xlsx
+++ b/dkjs.git.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="255" windowWidth="19395" windowHeight="7485" activeTab="12"/>
+    <workbookView xWindow="600" yWindow="255" windowWidth="19395" windowHeight="7485" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="b-测试" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="指数分析" sheetId="12" r:id="rId12"/>
     <sheet name="newSheet" sheetId="15" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="270">
   <si>
     <t>mRate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1043,6 +1043,34 @@
     <t>dfd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>罗龙6月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗龙7月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>罗龙8月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住宿报销6月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车费6月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车费7月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住宿报销7,8月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1056,7 +1084,7 @@
     <numFmt numFmtId="178" formatCode="0.0000%"/>
     <numFmt numFmtId="179" formatCode="#,##0.0_ "/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1105,6 +1133,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1513,6 +1548,40 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1551,40 +1620,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="31" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2797,10 +2832,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A2:P48"/>
+  <dimension ref="A2:P80"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41:I48"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3382,6 +3417,77 @@
       <c r="I48">
         <f>I46+I47</f>
         <v>782.7450000000008</v>
+      </c>
+    </row>
+    <row r="73" spans="8:13">
+      <c r="H73" t="s">
+        <v>267</v>
+      </c>
+      <c r="K73" s="40">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="74" spans="8:13">
+      <c r="H74" t="s">
+        <v>268</v>
+      </c>
+      <c r="K74" s="40">
+        <v>400</v>
+      </c>
+      <c r="M74" s="40"/>
+    </row>
+    <row r="75" spans="8:13">
+      <c r="H75" t="s">
+        <v>164</v>
+      </c>
+      <c r="K75" s="40">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="76" spans="8:13">
+      <c r="H76" t="s">
+        <v>263</v>
+      </c>
+      <c r="K76" s="40">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="77" spans="8:13">
+      <c r="H77" t="s">
+        <v>264</v>
+      </c>
+      <c r="K77" s="40">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="78" spans="8:13">
+      <c r="H78" t="s">
+        <v>265</v>
+      </c>
+      <c r="K78" s="40">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="79" spans="8:13">
+      <c r="H79" t="s">
+        <v>266</v>
+      </c>
+      <c r="K79">
+        <v>-1700</v>
+      </c>
+    </row>
+    <row r="80" spans="8:13">
+      <c r="H80" t="s">
+        <v>269</v>
+      </c>
+      <c r="K80" s="40">
+        <v>-2640</v>
+      </c>
+      <c r="L80">
+        <v>-500</v>
+      </c>
+      <c r="M80">
+        <v>-1900</v>
       </c>
     </row>
   </sheetData>
@@ -3577,7 +3683,7 @@
       <c r="N9" t="s">
         <v>225</v>
       </c>
-      <c r="O9" s="62">
+      <c r="O9" s="41">
         <v>42612</v>
       </c>
     </row>
@@ -3678,7 +3784,7 @@
         <f t="shared" ref="E15:E24" si="1">(D15-1000)/1000+1</f>
         <v>1.06372</v>
       </c>
-      <c r="S15" s="62"/>
+      <c r="S15" s="41"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16">
@@ -5478,88 +5584,88 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A4:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="4" spans="1:8">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="42" t="s">
         <v>255</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="42" t="s">
         <v>254</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="43" t="s">
         <v>257</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="43" t="s">
         <v>258</v>
       </c>
       <c r="B8" t="s">
         <v>259</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63" t="s">
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="64"/>
+      <c r="A9" s="43"/>
       <c r="B9" t="s">
         <v>259</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="64"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
+      <c r="A10" s="43"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
       <c r="H10" t="s">
         <v>257</v>
       </c>
@@ -5568,39 +5674,39 @@
       <c r="B11" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
         <v>260</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63" t="s">
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="G13" s="63"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
     </row>
     <row r="18" spans="3:9">
       <c r="C18" t="s">
@@ -34225,37 +34331,37 @@
       <c r="A1" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="43">
+      <c r="B1" s="54">
         <v>42258</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="50" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="51"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="62"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="24" t="s">
         <v>78</v>
       </c>
@@ -34265,10 +34371,10 @@
       <c r="E3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="53"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="24" t="s">
         <v>78</v>
       </c>
@@ -34277,7 +34383,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="50" t="s">
         <v>113</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -34291,7 +34397,7 @@
         <v>4.7799879114105722E-4</v>
       </c>
       <c r="E4" s="22"/>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="52" t="s">
         <v>85</v>
       </c>
       <c r="G4" s="22" t="s">
@@ -34306,7 +34412,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="55"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="26" t="s">
         <v>81</v>
       </c>
@@ -34316,7 +34422,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="22"/>
-      <c r="F5" s="42"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="22"/>
       <c r="H5" s="37"/>
       <c r="I5" s="33">
@@ -34325,7 +34431,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="55"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="26" t="s">
         <v>138</v>
       </c>
@@ -34339,7 +34445,7 @@
       <c r="E6" s="33">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F6" s="42"/>
+      <c r="F6" s="53"/>
       <c r="G6" s="22"/>
       <c r="H6" s="37"/>
       <c r="I6" s="33">
@@ -34348,7 +34454,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="55"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="26" t="s">
         <v>137</v>
       </c>
@@ -34358,7 +34464,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="42"/>
+      <c r="F7" s="53"/>
       <c r="G7" s="22"/>
       <c r="H7" s="37"/>
       <c r="I7" s="33">
@@ -34367,7 +34473,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="55"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="26"/>
       <c r="C8" s="37"/>
       <c r="D8" s="33">
@@ -34390,7 +34496,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="55"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="26"/>
       <c r="C9" s="37"/>
       <c r="D9" s="33">
@@ -34411,7 +34517,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="55"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="26"/>
       <c r="C10" s="37"/>
       <c r="D10" s="33">
@@ -34430,7 +34536,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="50" t="s">
         <v>114</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -34451,7 +34557,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="55"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="26" t="s">
         <v>83</v>
       </c>
@@ -34470,7 +34576,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="55"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="26" t="s">
         <v>134</v>
       </c>
@@ -34491,7 +34597,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="55"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="26" t="s">
         <v>135</v>
       </c>
@@ -34514,7 +34620,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="55"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="26" t="s">
         <v>133</v>
       </c>
@@ -34537,7 +34643,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="55"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="26" t="s">
         <v>136</v>
       </c>
@@ -34560,7 +34666,7 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="55"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="26" t="s">
         <v>139</v>
       </c>
@@ -34600,7 +34706,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="50" t="s">
         <v>115</v>
       </c>
       <c r="B19" s="26" t="s">
@@ -34621,7 +34727,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="55"/>
+      <c r="A20" s="51"/>
       <c r="B20" s="26" t="s">
         <v>107</v>
       </c>
@@ -34642,7 +34748,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="55"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="26"/>
       <c r="C21" s="37"/>
       <c r="D21" s="33">
@@ -34659,7 +34765,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.25" thickBot="1">
-      <c r="A22" s="55"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="26"/>
       <c r="C22" s="37"/>
       <c r="D22" s="33">
@@ -34676,10 +34782,10 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="B23" s="61"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="37">
         <f>SUM(C4:C22)</f>
         <v>4184111</v>
@@ -34688,10 +34794,10 @@
         <f>SUM(D4:D22)</f>
         <v>1</v>
       </c>
-      <c r="F23" s="58" t="s">
+      <c r="F23" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="G23" s="59"/>
+      <c r="G23" s="47"/>
       <c r="H23" s="37">
         <f>SUM(H4:H22)</f>
         <v>1095317</v>
@@ -34708,11 +34814,11 @@
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="35"/>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
     </row>
     <row r="25" spans="1:9" ht="14.25" thickBot="1">
       <c r="A25" s="30"/>
@@ -34723,12 +34829,12 @@
       <c r="F25" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G25" s="56">
+      <c r="G25" s="44">
         <f>C23-H23</f>
         <v>3088794</v>
       </c>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
@@ -34737,11 +34843,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A19:A22"/>
     <mergeCell ref="F4:F7"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="G24:I24"/>
@@ -34750,6 +34851,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A4:A10"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A19:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>